<commit_message>
Finished Step 5 and created coding scheme table
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E7DA06-ECDB-40B6-81EE-47B2FFEDC157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6775097-9365-42D5-8AAC-30C35A4B216D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>T0</t>
   </si>
@@ -266,6 +266,14 @@
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reorg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Re-organized data</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -616,7 +624,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -792,6 +800,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Update README and User Manual after Step 5
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6775097-9365-42D5-8AAC-30C35A4B216D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A865877-25F3-4DE0-816D-1E81BBD749BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>T0</t>
   </si>
@@ -274,6 +274,22 @@
   </si>
   <si>
     <t>Re-organized data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compare</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all avaiable waves in ABCD 5.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -624,7 +640,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -814,6 +830,12 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
@@ -821,7 +843,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="C15" s="3" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Re-constructing codes for Step 6 and fixed some bugs
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A865877-25F3-4DE0-816D-1E81BBD749BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B66D234-9CF0-4190-8CAF-73151A211C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>T0</t>
   </si>
@@ -98,210 +98,229 @@
   </si>
   <si>
     <t>Rep</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Auto-generated Report</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Rec</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Raw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Raw data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of Account</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>NOA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ODQ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Online Dating Questionnaire</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Imp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Imputed data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Re-coded data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SMAS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>bergen Social Media Addiction Scale</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>VGAS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Video Game Addiction Scale</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>MPIQ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone Involvement Questionnaire</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Common</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Novel Technology</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SMQ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Social Media Questionnaire</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>UM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Use Most</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowErs</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>NOFE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>NOFI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowIngs</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TPD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SOCial media apps</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>weekday</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>weekend</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekday</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekend day</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>School</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>School-related work</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>calculated value from open-answered STQ items</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TPW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Time Per Week</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TyPical Day (prefix) or Time Per Day (postfix)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SUAB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Reorg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Re-organized data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Comp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Compare</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ALL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>all avaiable waves in ABCD 5.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summary</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mental Health</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -393,21 +412,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -637,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -858,6 +883,12 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>50</v>
       </c>
@@ -865,7 +896,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17.25" x14ac:dyDescent="0.2">
       <c r="C17" s="3" t="s">
         <v>51</v>
       </c>
@@ -873,7 +904,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
@@ -881,7 +912,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
@@ -889,7 +920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.25" x14ac:dyDescent="0.2">
       <c r="C20" s="3" t="s">
         <v>41</v>
       </c>
@@ -897,7 +928,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="3:4" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17.25" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
@@ -905,7 +936,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.25" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>32</v>
       </c>
@@ -913,7 +944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="3:4" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17.25" x14ac:dyDescent="0.2">
       <c r="C23" s="3" t="s">
         <v>66</v>
       </c>
@@ -921,12 +952,19 @@
         <v>67</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Step 7 and updated relevant documents
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3930B216-E8B6-4981-AD76-BB256161FCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97B069-642F-453B-A5A0-F720F20E07EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,571 +20,793 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
   <si>
     <t>Rep</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Rec</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Raw</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Raw data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of Account</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>NOA</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>ODQ</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Online Dating Questionnaire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Imp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Imputed data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Re-coded data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SMAS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>bergen Social Media Addiction Scale</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>VGAS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Video Game Addiction Scale</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>MPIQ</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone Involvement Questionnaire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Common</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Novel Technology</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SMQ</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Social Media Questionnaire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Use Most</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowErs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>NOFE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>NOFI</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowIngs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>TPD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SOCial media apps</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>weekday</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>weekend</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekday</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekend day</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>School</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>School-related work</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>calculated value from open-answered STQ items</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>TPW</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Time Per Week</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>TyPical Day (prefix) or Time Per Day (postfix)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SUAB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Reorg</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Re-organized data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Comp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Compare</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>ALL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>all avaiable waves in ABCD 5.0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>S</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Mental Health</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Children Short Form (ABCD-version)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_NU</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_SS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BIS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Inhibition System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BAS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Activation System (Subscale in BIS/BAS)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BAS_FS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Fun Seeking (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BAS_Drive</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Drive (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BAS_RR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Reward Responsiveness (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Sum</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Sum Scores (when as postfix of variable names)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PEQ</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Peer Experiences Questionnaire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Overt</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Overt Aggression or Victimization</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Rel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Relational Aggression or Victimization</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Reputational Aggression or Victimization</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Agg</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Aggression</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Vic</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Victimization</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PPS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Prodromal Psychosis Scale</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Sum</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - Total number of youth-reported psychotic-like experiences</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - The severity score of PPS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Mania </t>
   </si>
   <si>
     <t>7-Up Mania Inventory</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Summary (when as postfix of files)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Negative Urgency (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Planning (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPlan</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Perseverance(Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_PU</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Positive Urgency (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Sensation Seeking (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity_Mean</t>
   </si>
   <si>
     <t>PPS Derivatives - The mean severity score of PPS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Youth-reported Life Events</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good_Affected</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad_Affected</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of bad events</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of good events</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of good events</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of bad events</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>T0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SMA</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Screen Media Activity</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>T1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>OS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>OwnerShip</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>T2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>STQ</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Screen Time Questionnaire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>T3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>T4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>MVA</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Missing Value Analysis</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>MI</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Multiple Imputation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SOC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>MVOC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Multiplayer Videogame Online Chatting</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>MP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>One-year follow-up wave</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Two-year follow-up wave</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Three-year follow-up wave</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Four-year follow-up wave</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Baseline wave</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>auto-generated Report</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>MH</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>ERQ</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Emotion Regulation Questionnaire</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Reappraisal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: reapprasial (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: Suppression (Sum Score)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Suppression</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parent-reported About Youth</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Youth Self-reported</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Child Behavior Checklist</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASEBA Measures</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thought</t>
+  </si>
+  <si>
+    <t>CBCL Syndrome Scale - Thought Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attention</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Syndrome Scale - Attention Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RuleBreak</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aggressive</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Internal</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Composite Score - Internealizing Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>External</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Composite Score - Externalizing Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotProb</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Composite Score - Total Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Depress</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anxitey</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL DSM-5-Oriented Scale - Anxiety Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL DSM-5-Oriented Scale - Somatic Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADHD</t>
+  </si>
+  <si>
+    <t>CBCL DSM-5-Oriented Scale - Attention Deficit/Hyperactivity Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Opposite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL DSM-5-Oriented Scale - Oppositional Defiant Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conduct</t>
+  </si>
+  <si>
+    <t>CBCL DSM-5-Oriented Scale - Conduct Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASEBA</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Achenbach System of Empirically Based Assessment</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Syndrome Scale - Aggressive Behavior</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Syndrome Scale - Rule-breaking Behavior</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Syndrome Scale - Social Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SomaticPr</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SomaticCo</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>WithDep</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Syndrome Scale - Withdrawn/Depressed</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Syndrome Scale - Somatic Complaints</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnxDep</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL Syndrom Scale - Anxious/Depressed</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCT</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>OCD</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stress</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL 2007 Scale - Sluggish Cognitive Tempo</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL 2007 Scale - Obsessive-Compulsive Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL DSM-5-Oriented Scale - Affective Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBCL 2007 Scale - Post-traumatic Stress Problems</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>VSO</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable-values Summary Overview</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -660,29 +882,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -913,26 +1141,26 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.75" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -952,7 +1180,7 @@
       <c r="A3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>126</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1033,11 +1261,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>131</v>
+      <c r="A9" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>189</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>34</v>
@@ -1048,10 +1276,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>19</v>
@@ -1062,10 +1290,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>121</v>
@@ -1076,10 +1304,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
@@ -1090,10 +1318,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>122</v>
@@ -1104,10 +1332,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>21</v>
@@ -1118,10 +1346,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>24</v>
@@ -1132,10 +1360,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>25</v>
@@ -1146,10 +1374,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>5</v>
@@ -1160,10 +1388,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>124</v>
@@ -1173,11 +1401,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>49</v>
+      <c r="A19" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>15</v>
@@ -1187,8 +1415,12 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>142</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>13</v>
       </c>
@@ -1197,8 +1429,12 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>6</v>
       </c>
@@ -1207,8 +1443,12 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>40</v>
       </c>
@@ -1217,32 +1457,38 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="7" t="s">
+      <c r="A23" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="14"/>
       <c r="C26" s="4" t="s">
         <v>58</v>
       </c>
@@ -1251,6 +1497,12 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="C27" s="5" t="s">
         <v>60</v>
       </c>
@@ -1259,6 +1511,12 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>180</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>62</v>
       </c>
@@ -1267,14 +1525,26 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C29" s="9" t="s">
+      <c r="A29" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>178</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>68</v>
       </c>
@@ -1283,6 +1553,12 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>173</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>70</v>
       </c>
@@ -1291,6 +1567,12 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="C32" s="5" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1580,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>149</v>
+      </c>
       <c r="C33" s="5" t="s">
         <v>73</v>
       </c>
@@ -1306,7 +1594,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>171</v>
+      </c>
       <c r="C34" s="5" t="s">
         <v>75</v>
       </c>
@@ -1314,15 +1608,27 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" s="9" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="3:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>153</v>
+      </c>
       <c r="C36" s="5" t="s">
         <v>79</v>
       </c>
@@ -1330,7 +1636,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="C37" s="5" t="s">
         <v>81</v>
       </c>
@@ -1338,7 +1650,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>157</v>
+      </c>
       <c r="C38" s="5" t="s">
         <v>94</v>
       </c>
@@ -1346,15 +1664,27 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>186</v>
+      </c>
       <c r="C39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>160</v>
+      </c>
       <c r="C40" s="2" t="s">
         <v>50</v>
       </c>
@@ -1362,7 +1692,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>161</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>88</v>
       </c>
@@ -1370,7 +1706,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>163</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>89</v>
       </c>
@@ -1378,7 +1720,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="C43" s="2" t="s">
         <v>52</v>
       </c>
@@ -1386,7 +1734,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>167</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>91</v>
       </c>
@@ -1394,7 +1748,13 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="C45" s="3" t="s">
         <v>53</v>
       </c>
@@ -1402,15 +1762,27 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C46" s="9" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="C47" s="5" t="s">
         <v>98</v>
       </c>
@@ -1418,7 +1790,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C48" s="5" t="s">
         <v>99</v>
       </c>
@@ -1443,10 +1815,10 @@
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="8" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1467,12 +1839,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Start re-constructing Step 8 & Update documents
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97B069-642F-453B-A5A0-F720F20E07EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A359B17-B561-427E-B9DD-123877922626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,772 +20,1035 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="256">
   <si>
     <t>Rep</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Rec</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Raw</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Raw data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of Account</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>NOA</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ODQ</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Online Dating Questionnaire</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Imp</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Imputed data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Re-coded data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SMAS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>bergen Social Media Addiction Scale</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>VGAS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Video Game Addiction Scale</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>MPIQ</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone Involvement Questionnaire</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Common</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Novel Technology</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SMQ</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Social Media Questionnaire</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UM</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Use Most</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowErs</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>NOFE</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>NOFI</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowIngs</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>TPD</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SOCial media apps</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>weekday</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>weekend</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekday</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekend day</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>School</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>School-related work</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>calculated value from open-answered STQ items</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>TPW</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Time Per Week</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>TyPical Day (prefix) or Time Per Day (postfix)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SUAB</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Reorg</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Re-organized data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Comp</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Compare</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ALL</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>all avaiable waves in ABCD 5.0</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>S</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Mental Health</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Children Short Form (ABCD-version)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_NU</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_SS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BIS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Inhibition System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BAS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Activation System (Subscale in BIS/BAS)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BAS_FS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Fun Seeking (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BAS_Drive</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Drive (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BAS_RR</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Reward Responsiveness (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Sum</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Sum Scores (when as postfix of variable names)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PEQ</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Peer Experiences Questionnaire</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Overt</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Overt Aggression or Victimization</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Rel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Relational Aggression or Victimization</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Reputational Aggression or Victimization</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Agg</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Aggression</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Vic</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Victimization</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PPS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Prodromal Psychosis Scale</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Sum</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - Total number of youth-reported psychotic-like experiences</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - The severity score of PPS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Mania </t>
   </si>
   <si>
     <t>7-Up Mania Inventory</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Summary (when as postfix of files)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Negative Urgency (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Planning (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPers</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPlan</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Perseverance(Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_PU</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Positive Urgency (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Sensation Seeking (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity_Mean</t>
   </si>
   <si>
     <t>PPS Derivatives - The mean severity score of PPS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Youth-reported Life Events</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good_Affected</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad_Affected</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of bad events</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of good events</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of good events</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of bad events</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>T0</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SMA</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Screen Media Activity</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>T1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>OS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>OwnerShip</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>T2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>STQ</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Screen Time Questionnaire</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>T3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>T4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>MVA</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Missing Value Analysis</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>MI</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Multiple Imputation</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SOC</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>MVOC</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Multiplayer Videogame Online Chatting</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>MP</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>One-year follow-up wave</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Two-year follow-up wave</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Three-year follow-up wave</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Four-year follow-up wave</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Baseline wave</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>auto-generated Report</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>MH</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ERQ</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Emotion Regulation Questionnaire</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Reappraisal</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: reapprasial (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: Suppression (Sum Score)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Suppression</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>P</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Parent-reported About Youth</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Youth Self-reported</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Child Behavior Checklist</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ASEBA Measures</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Thought</t>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Thought Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Attention</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Attention Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>RuleBreak</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Aggressive</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Internal</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Internealizing Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>External</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Externalizing Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>TotProb</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Total Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Depress</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Anxitey</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Anxiety Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Somatic Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ADHD</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Attention Deficit/Hyperactivity Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Opposite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Oppositional Defiant Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Conduct</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Conduct Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ASEBA</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Achenbach System of Empirically Based Assessment</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Aggressive Behavior</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Rule-breaking Behavior</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Social</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Social Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SomaticPr</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SomaticCo</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>WithDep</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Withdrawn/Depressed</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Somatic Complaints</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>AnxDep</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrom Scale - Anxious/Depressed</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SCT</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>OCD</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Stress</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Sluggish Cognitive Tempo</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Obsessive-Compulsive Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Affective Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Post-traumatic Stress Problems</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>VSO</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Variable-values Summary Overview</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neuro-Cognition</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SU</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magnetic Resonance Imaging</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>rsfMRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resting-state functional MRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>tfMRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task-based functional MRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>sMRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Structural MRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diffusion MRI - Diffusion Tensor Imaging</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diffusion MRI - Restriction Spectrum Imaging</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quality Control of MRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imaging-related Variables</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecInc</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recommended Image Inclusion</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>HM</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Head Motion</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeanFD</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean Frame-wise Displacement</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MID</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monetary Incentive Delay task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SST</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stop Signal Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enback</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotional N-back task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behav</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behavioral Performance during task-based fMRI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>QC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSFNC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resting-state Functional canonical Network Connectivity</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Culture and Environment</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PH</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Physical Health</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Substance Use</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ge</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genetics</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked External Data</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neurocognition</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>NIHTB</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>The NIH Cognition Toolbox</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PVT</t>
+  </si>
+  <si>
+    <t>Picture Vocabulary Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>FICAT</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PSMT</t>
+  </si>
+  <si>
+    <t>DCCST</t>
+  </si>
+  <si>
+    <t>PCST</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORRT</t>
+  </si>
+  <si>
+    <t>LSWMT</t>
+  </si>
+  <si>
+    <t>Fluid</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Cryst</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crystalized Intelligence Composite Score</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fluid Intelligence Composite Score</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Intelligence Composite Score</t>
+  </si>
+  <si>
+    <t>Flanker Inhibitory Control &amp; Attention Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> List Sorting Working Memory Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oral Reading Recognition Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pattern Comparison processing Speed Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dimensional Change Card Sort Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture Sequence Memory Task</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -882,35 +1145,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1138,31 +1403,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.75" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>106</v>
       </c>
@@ -1175,8 +1446,14 @@
       <c r="D2" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>109</v>
       </c>
@@ -1189,8 +1466,14 @@
       <c r="D3" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>112</v>
       </c>
@@ -1203,8 +1486,14 @@
       <c r="D4" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>115</v>
       </c>
@@ -1217,8 +1506,14 @@
       <c r="D5" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>116</v>
       </c>
@@ -1232,7 +1527,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>117</v>
       </c>
@@ -1245,8 +1540,14 @@
       <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>119</v>
       </c>
@@ -1260,11 +1561,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>189</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1274,7 +1575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -1288,7 +1589,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -1302,7 +1603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -1316,7 +1617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1330,7 +1631,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -1344,7 +1645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
@@ -1357,8 +1658,14 @@
       <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -1371,8 +1678,14 @@
       <c r="D16" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>48</v>
       </c>
@@ -1386,7 +1699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>64</v>
       </c>
@@ -1400,7 +1713,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>139</v>
       </c>
@@ -1414,7 +1727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>141</v>
       </c>
@@ -1428,7 +1741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>107</v>
       </c>
@@ -1441,8 +1754,14 @@
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>132</v>
       </c>
@@ -1455,40 +1774,78 @@
       <c r="D22" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E22" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>168</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="15"/>
+      <c r="E23" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="C24" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>194</v>
+      </c>
       <c r="C25" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B26" s="14"/>
+      <c r="E25" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>225</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>58</v>
       </c>
@@ -1496,12 +1853,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>144</v>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>60</v>
@@ -1510,12 +1867,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>180</v>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>228</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>62</v>
@@ -1524,12 +1881,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>177</v>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>66</v>
@@ -1538,12 +1895,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>178</v>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>232</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>68</v>
@@ -1552,13 +1909,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>173</v>
-      </c>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C31" s="5" t="s">
         <v>70</v>
       </c>
@@ -1566,13 +1917,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>146</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>147</v>
-      </c>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C32" s="5" t="s">
         <v>0</v>
       </c>
@@ -1580,13 +1925,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>149</v>
-      </c>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C33" s="5" t="s">
         <v>73</v>
       </c>
@@ -1594,13 +1933,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>171</v>
-      </c>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C34" s="5" t="s">
         <v>75</v>
       </c>
@@ -1608,13 +1941,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>170</v>
-      </c>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B35" s="15"/>
       <c r="C35" s="7" t="s">
         <v>77</v>
       </c>
@@ -1622,12 +1953,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>153</v>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>235</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>79</v>
@@ -1636,12 +1967,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>155</v>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>237</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>81</v>
@@ -1650,12 +1981,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>157</v>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>250</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>94</v>
@@ -1664,12 +1995,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>186</v>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>239</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>255</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>83</v>
@@ -1678,12 +2009,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>160</v>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>240</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>254</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>50</v>
@@ -1692,12 +2023,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>161</v>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>253</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>88</v>
@@ -1706,12 +2037,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>162</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>163</v>
+        <v>242</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>89</v>
@@ -1720,12 +2051,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>165</v>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>251</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>52</v>
@@ -1734,12 +2065,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>166</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>167</v>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>247</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>91</v>
@@ -1748,12 +2079,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>184</v>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>248</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>53</v>
@@ -1762,12 +2093,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>185</v>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>245</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>249</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>97</v>
@@ -1775,22 +2106,29 @@
       <c r="D46" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>187</v>
-      </c>
+      <c r="E46" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C47" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="16"/>
       <c r="C48" s="5" t="s">
         <v>99</v>
       </c>
@@ -1798,7 +2136,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="16"/>
       <c r="C49" s="5" t="s">
         <v>100</v>
       </c>
@@ -1806,7 +2145,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="16"/>
       <c r="C50" s="5" t="s">
         <v>101</v>
       </c>
@@ -1814,7 +2154,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="16"/>
       <c r="C51" s="8" t="s">
         <v>133</v>
       </c>
@@ -1822,7 +2163,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C52" s="5" t="s">
         <v>135</v>
       </c>
@@ -1830,7 +2171,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C53" s="5" t="s">
         <v>138</v>
       </c>
@@ -1838,14 +2179,190 @@
         <v>137</v>
       </c>
     </row>
+    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C54" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="15"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C61" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C62" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C63" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C64" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C65" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C67" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C68" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C69" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>166</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Step 8 & Update Documents
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A359B17-B561-427E-B9DD-123877922626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E472867-98B5-47E1-A2CF-A47D23613C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1171,11 +1172,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1403,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1420,18 +1421,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1446,10 +1447,10 @@
       <c r="D2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>205</v>
       </c>
     </row>
@@ -1466,10 +1467,10 @@
       <c r="D3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>208</v>
       </c>
     </row>
@@ -1486,10 +1487,10 @@
       <c r="D4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1506,10 +1507,10 @@
       <c r="D5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1526,6 +1527,12 @@
       <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="E6" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -1540,11 +1547,11 @@
       <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>200</v>
+      <c r="E7" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1560,6 +1567,12 @@
       <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="E8" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
@@ -1574,6 +1587,12 @@
       <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="E9" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -1588,6 +1607,12 @@
       <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E10" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -1602,6 +1627,12 @@
       <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="E11" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -1616,6 +1647,12 @@
       <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="E12" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -1630,6 +1667,12 @@
       <c r="D13" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="E13" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -1644,6 +1687,12 @@
       <c r="D14" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E14" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -1658,11 +1707,11 @@
       <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>196</v>
+      <c r="E15" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1678,14 +1727,8 @@
       <c r="D16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>48</v>
       </c>
@@ -1699,7 +1742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>64</v>
       </c>
@@ -1713,7 +1756,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>139</v>
       </c>
@@ -1727,7 +1770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>141</v>
       </c>
@@ -1741,7 +1784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>107</v>
       </c>
@@ -1754,14 +1797,8 @@
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>132</v>
       </c>
@@ -1774,596 +1811,565 @@
       <c r="D22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>168</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C31" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C32" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C33" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C34" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>239</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>240</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>242</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>243</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>244</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>245</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C47" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="16"/>
-      <c r="C48" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="16"/>
-      <c r="C49" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="16"/>
-      <c r="C50" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="16"/>
-      <c r="C51" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C52" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C53" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C54" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C55" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C56" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C57" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C58" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C59" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>146</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C61" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C62" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C63" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C64" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C65" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C66" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C67" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C68" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C69" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C70" t="s">
-        <v>162</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C71" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C72" t="s">
-        <v>166</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C73" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C74" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C75" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>187</v>
-      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="15"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="15"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="15"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C54:D54"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD99DF5-9F47-4A74-87B4-59EB099EE2E2}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="66.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C15" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Step 9 & 10, User Manual and README
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C4F880-BE3B-4853-AA0D-A2891DDF0AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBE0D5-B617-4AD1-9082-0507FAC74130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="291">
   <si>
     <t>Rep</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -243,10 +243,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>Behavioral Activation System (Subscale in BIS/BAS)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>BAS_FS</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -291,22 +287,10 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>PEQ Subscale - Overt Aggression or Victimization</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>Rel</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>PEQ Subscale - Relational Aggression or Victimization</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEQ Subscale - Reputational Aggression or Victimization</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>Agg</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -870,14 +854,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>Enback</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emotional N-back task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>Behav</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -1171,6 +1147,30 @@
   </si>
   <si>
     <t>Abbr NC</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>NB</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>emotional N-Back task</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behavioral Activation System (subscale in BIS/BAS)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEQ Subscale - Relational (Aggression or Victimization)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEQ Subscale - Reputational (Aggression or Victimization)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEQ Subscale - Overt (Aggression or Victimization)</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -1178,7 +1178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1271,11 +1271,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF444444"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1312,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1350,8 +1345,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1580,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E10" sqref="E10:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1598,70 +1594,70 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>203</v>
+        <v>108</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
@@ -1670,18 +1666,18 @@
         <v>37</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>35</v>
@@ -1690,18 +1686,18 @@
         <v>36</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>26</v>
@@ -1710,18 +1706,18 @@
         <v>34</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>28</v>
@@ -1730,18 +1726,18 @@
         <v>30</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>29</v>
@@ -1750,18 +1746,18 @@
         <v>31</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>32</v>
@@ -1770,10 +1766,10 @@
         <v>33</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1781,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
@@ -1790,10 +1786,10 @@
         <v>18</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1804,16 +1800,16 @@
         <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1829,11 +1825,11 @@
       <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>214</v>
+      <c r="E12" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1844,16 +1840,16 @@
         <v>3</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1870,10 +1866,10 @@
         <v>20</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1890,10 +1886,10 @@
         <v>21</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1915,7 +1911,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>5</v>
@@ -1925,25 +1921,25 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>63</v>
+      <c r="A18" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>15</v>
@@ -1953,11 +1949,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>140</v>
+      <c r="A20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>13</v>
@@ -1968,10 +1964,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>6</v>
@@ -1981,11 +1977,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>47</v>
+      <c r="A22" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>38</v>
@@ -1995,68 +1991,71 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>166</v>
+      <c r="A23" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>228</v>
-      </c>
+      <c r="A30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="15"/>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="15"/>
@@ -2066,9 +2065,6 @@
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" s="15"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -2082,7 +2078,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2097,350 +2093,350 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="24" t="s">
         <v>53</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>55</v>
+      <c r="D3" s="24" t="s">
+        <v>287</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>290</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>288</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>70</v>
+      <c r="D10" s="23" t="s">
+        <v>289</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>48</v>
@@ -2449,189 +2445,206 @@
         <v>49</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>180</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>206</v>
+      </c>
       <c r="C27" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B28" s="23"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>208</v>
+      </c>
       <c r="C28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>286</v>
+      </c>
       <c r="C29" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="21"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C31" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Step 10 & Update LICENSE
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBE0D5-B617-4AD1-9082-0507FAC74130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DEA7E5-B798-4AD0-8612-164AE9A74747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,916 +21,916 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="295">
   <si>
     <t>Rep</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Rec</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Raw</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Raw data</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of Account</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NOA</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ODQ</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Online Dating Questionnaire</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Imp</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Imputed data</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Re-coded data</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SMAS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>bergen Social Media Addiction Scale</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>VGAS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Video Game Addiction Scale</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MPIQ</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone Involvement Questionnaire</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SMQ</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Social Media Questionnaire</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UM</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Use Most</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowErs</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NOFE</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NOFI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowIngs</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>TPD</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SOCial media apps</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>weekday</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>weekend</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekday</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekend day</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>School</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>School-related work</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>calculated value from open-answered STQ items</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>TPW</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Time Per Week</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>TyPical Day (prefix) or Time Per Day (postfix)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SUAB</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Reorg</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Re-organized data</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Comp</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Compare</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ALL</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>all avaiable waves in ABCD 5.0</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>S</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Mental Health</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Children Short Form (ABCD-version)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_NU</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_SS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BIS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Inhibition System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BAS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BAS_FS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Fun Seeking (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BAS_Drive</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Drive (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BAS_RR</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Reward Responsiveness (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Sum</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Sum Scores (when as postfix of variable names)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PEQ</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Peer Experiences Questionnaire</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Overt</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Rel</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Agg</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Aggression</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Vic</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Victimization</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PPS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Prodromal Psychosis Scale</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Sum</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - Total number of youth-reported psychotic-like experiences</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - The severity score of PPS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Mania </t>
   </si>
   <si>
     <t>7-Up Mania Inventory</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Summary (when as postfix of files)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Negative Urgency (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Planning (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPers</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPlan</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Perseverance(Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_PU</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Positive Urgency (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Sensation Seeking (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity_Mean</t>
   </si>
   <si>
     <t>PPS Derivatives - The mean severity score of PPS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Youth-reported Life Events</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good_Affected</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad_Affected</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of bad events</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of good events</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of good events</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of bad events</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>T0</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SMA</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Screen Media Activity</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>T1</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>OS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>OwnerShip</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>T2</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>STQ</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Screen Time Questionnaire</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>T3</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>T4</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MVA</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Missing Value Analysis</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Multiple Imputation</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SOC</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MVOC</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Multiplayer Videogame Online Chatting</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MP</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>One-year follow-up wave</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Two-year follow-up wave</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Three-year follow-up wave</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Four-year follow-up wave</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Baseline wave</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>auto-generated Report</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MH</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ERQ</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Emotion Regulation Questionnaire</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Reappraisal</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: reapprasial (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: Suppression (Sum Score)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Suppression</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>P</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Parent-reported About Youth</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Youth Self-reported</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Child Behavior Checklist</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Thought</t>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Thought Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Attention</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Attention Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>RuleBreak</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Aggressive</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Internal</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Internealizing Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>External</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Externalizing Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>TotProb</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Total Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Depress</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Anxitey</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Anxiety Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Somatic Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ADHD</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Attention Deficit/Hyperactivity Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Opposite</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Oppositional Defiant Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Conduct</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Conduct Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ASEBA</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Achenbach System of Empirically Based Assessment</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Aggressive Behavior</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Rule-breaking Behavior</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Social</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Social Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SomaticPr</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SomaticCo</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>WithDep</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Withdrawn/Depressed</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Somatic Complaints</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>AnxDep</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrom Scale - Anxious/Depressed</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SCT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>OCD</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Stress</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Sluggish Cognitive Tempo</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Obsessive-Compulsive Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Affective Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Post-traumatic Stress Problems</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>VSO</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Variable-values Summary Overview</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NC</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Neuro-Cognition</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SU</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Magnetic Resonance Imaging</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>rsfMRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state functional MRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>tfMRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Task-based functional MRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>sMRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Structural MRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>DTI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Diffusion Tensor Imaging</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>RSI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Restriction Spectrum Imaging</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Quality Control of MRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>RecInc</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Recommended Image Inclusion</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>HM</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Head Motion</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MeanFD</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Mean Frame-wise Displacement</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MID</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Monetary Incentive Delay task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SST</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Stop Signal Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Behav</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Performance during task-based fMRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>QC</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>RSFNC</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state Functional canonical Network Connectivity</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CE</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Culture and Environment</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PH</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Physical Health</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Substance Use</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Ge</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Genetics</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>LED</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Linked External Data</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NIHTB</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>The NIH Cognition Toolbox</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PVT</t>
   </si>
   <si>
     <t>Picture Vocabulary Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>FICAT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PSMT</t>
@@ -940,7 +940,7 @@
   </si>
   <si>
     <t>PCST</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ORRT</t>
@@ -956,233 +956,256 @@
   </si>
   <si>
     <t>Cryst</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Crystalized Intelligence Composite Score</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Fluid Intelligence Composite Score</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Total Intelligence Composite Score</t>
   </si>
   <si>
     <t>Flanker Inhibitory Control &amp; Attention Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> List Sorting Working Memory Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Oral Reading Recognition Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Pattern Comparison processing Speed Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Dimensional Change Card Sort Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Picture Sequence Memory Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Non-NIHTB</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognitive Task exlcuding NIH toolbox</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>CCT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Cash Choice Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>LMT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Little Man Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>RAVLT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>the pearson Rey Auditory Verbal Learning Test</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>WISC</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Wechsler Intelligence Scale for Children (5th Ed.) - Martix Reasoning</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>DDT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Delay Discounting Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EST</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Emotional Stroop Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>GDT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Game of Dice Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SIT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Social Influence Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SMART</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Stanford Mental Arithmetic Response Time Evaluation</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>BIRD</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Indicator of Resiliency to Distress Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MFT</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Millisecond Flanker Task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NAA</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition Assessment Administration</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SVS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Snellen Visual Screener</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Common</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SDPP Derivatives File Name</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Novel Technology</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ABCD MRI-related Measures</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MRI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Screen</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Youth Mental Health Summary</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>ABCD ASEBA Measures</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Abbr ASEBA</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MHS</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Abbr NC</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NB</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>emotional N-Back task</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Activation System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Relational (Aggression or Victimization)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Reputational (Aggression or Victimization)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Overt (Aggression or Victimization)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>MID-PQ</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post scan Questionnaire after MID task</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>RECMEM</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>N-Back Recognition Memory task</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1307,48 +1330,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1578,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2067,7 +2092,7 @@
       <c r="B46" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2077,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD99DF5-9F47-4A74-87B4-59EB099EE2E2}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2630,8 +2655,12 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
-      <c r="B30" s="23"/>
+      <c r="A30" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>129</v>
       </c>
@@ -2640,6 +2669,12 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>294</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>132</v>
       </c>
@@ -2648,7 +2683,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update for Step 11
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD0ACA7-7959-4391-B221-6F0D6A226694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A6202-4B3A-468F-89B6-561E9C31D01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17535" yWindow="4740" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,900 +22,900 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="340">
   <si>
     <t>Rep</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Rec</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Raw</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Raw data</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of Account</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>NOA</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ODQ</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Online Dating Questionnaire</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Imp</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Imputed data</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Re-coded data</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SMAS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>bergen Social Media Addiction Scale</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>VGAS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Video Game Addiction Scale</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MPIQ</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone Involvement Questionnaire</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SMQ</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Social Media Questionnaire</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UM</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Use Most</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowErs</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>NOFE</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>NOFI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowIngs</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>TPD</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SOCial media apps</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>weekday</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>weekend</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekday</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekend day</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>School</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>School-related work</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>calculated value from open-answered STQ items</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>TPW</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Time Per Week</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>TyPical Day (prefix) or Time Per Day (postfix)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SUAB</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Reorg</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Re-organized data</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Comp</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Compare</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ALL</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>all avaiable waves in ABCD 5.0</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>S</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Mental Health</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Children Short Form (ABCD-version)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_NU</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_SS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BIS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Inhibition System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BAS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BAS_FS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Fun Seeking (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BAS_Drive</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Drive (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BAS_RR</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Reward Responsiveness (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Sum</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Sum Scores (when as postfix of variable names)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Peer Experiences Questionnaire</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Agg</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Vic</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PPS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Prodromal Psychosis Scale</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Sum</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - Total number of youth-reported psychotic-like experiences</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - The severity score of PPS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Mania </t>
   </si>
   <si>
     <t>7-Up Mania Inventory</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Summary (when as postfix of files)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Negative Urgency (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Planning (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPers</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPlan</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Perseverance(Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_PU</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Positive Urgency (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Sensation Seeking (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity_Mean</t>
   </si>
   <si>
     <t>PPS Derivatives - The mean severity score of PPS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Youth-reported Life Events</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good_Affected</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad_Affected</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of bad events</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of good events</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of good events</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of bad events</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>T0</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SMA</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Screen Media Activity</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>T1</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>OS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>OwnerShip</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>T2</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>STQ</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Screen Time Questionnaire</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>T3</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>T4</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MVA</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Missing Value Analysis</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Multiple Imputation</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SOC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MVOC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Multiplayer Videogame Online Chatting</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MP</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>One-year follow-up wave</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Two-year follow-up wave</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Three-year follow-up wave</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Four-year follow-up wave</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Baseline wave</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>auto-generated Report</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MH</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ERQ</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Emotion Regulation Questionnaire</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Reappraisal</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: reapprasial (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: Suppression (Sum Score)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Suppression</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>P</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Parent-reported About Youth</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Youth Self-reported</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Child Behavior Checklist</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Thought</t>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Thought Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Attention</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Attention Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>RuleBreak</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Aggressive</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Internal</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Internealizing Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>External</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Externalizing Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>TotProb</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Total Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Depress</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Anxitey</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Anxiety Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Somatic Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ADHD</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Attention Deficit/Hyperactivity Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Opposite</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Oppositional Defiant Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Conduct</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Conduct Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ASEBA</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Achenbach System of Empirically Based Assessment</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Aggressive Behavior</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Rule-breaking Behavior</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Social</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Social Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SomaticPr</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SomaticCo</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>WithDep</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Withdrawn/Depressed</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Somatic Complaints</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>AnxDep</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrom Scale - Anxious/Depressed</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SCT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>OCD</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Stress</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Sluggish Cognitive Tempo</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Obsessive-Compulsive Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Affective Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Post-traumatic Stress Problems</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>VSO</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Variable-values Summary Overview</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>NC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Neuro-Cognition</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SU</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Magnetic Resonance Imaging</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>rsfMRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state functional MRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>tfMRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Task-based functional MRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>sMRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Structural MRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>DTI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Diffusion Tensor Imaging</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>RSI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Restriction Spectrum Imaging</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Quality Control of MRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>RecInc</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Recommended Image Inclusion</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>HM</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Head Motion</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MeanFD</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Mean Frame-wise Displacement</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MID</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Monetary Incentive Delay task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SST</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Stop Signal Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Behav</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Performance during task-based fMRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>QC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>RSFNC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state Functional canonical Network Connectivity</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CE</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Culture and Environment</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PH</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Physical Health</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Substance Use</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Ge</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Genetics</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>LED</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Linked External Data</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>NIHTB</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>The NIH Cognition Toolbox</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PVT</t>
   </si>
   <si>
     <t>Picture Vocabulary Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>FICAT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PSMT</t>
@@ -925,7 +925,7 @@
   </si>
   <si>
     <t>PCST</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ORRT</t>
@@ -941,309 +941,452 @@
   </si>
   <si>
     <t>Cryst</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Crystalized Intelligence Composite Score</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Fluid Intelligence Composite Score</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Total Intelligence Composite Score</t>
   </si>
   <si>
     <t>Flanker Inhibitory Control &amp; Attention Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> List Sorting Working Memory Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Oral Reading Recognition Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Pattern Comparison processing Speed Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Dimensional Change Card Sort Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Picture Sequence Memory Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Non-NIHTB</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognitive Task exlcuding NIH toolbox</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>CCT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Cash Choice Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>LMT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Little Man Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>RAVLT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>the pearson Rey Auditory Verbal Learning Test</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>WISC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Wechsler Intelligence Scale for Children (5th Ed.) - Martix Reasoning</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>DDT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Delay Discounting Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>EST</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Emotional Stroop Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>GDT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Game of Dice Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SIT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Social Influence Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SMART</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Stanford Mental Arithmetic Response Time Evaluation</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BIRD</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Indicator of Resiliency to Distress Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Millisecond Flanker Task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>NAA</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition Assessment Administration</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SVS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Snellen Visual Screener</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Common</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>SDPP Derivatives File Name</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Novel Technology</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ABCD MRI-related Measures</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MRI</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Screen</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Youth Mental Health Summary</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ABCD ASEBA Measures</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Abbr ASEBA</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MHS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Abbr NC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>NB</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>emotional N-Back task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Activation System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Relational (Aggression or Victimization)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Reputational (Aggression or Victimization)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Overt (Aggression or Victimization)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>RECMEM</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>N-Back Recognition Memory task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MIDPQ</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Post-scan Questionnaire after MID task</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>FLKR</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>BDEFS</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Barkely Deficits in Executive Functioning Scale</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Overt</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Rel</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Rep</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Aggression (only as postfix)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Victimization (only as postfix)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Abbr CE</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Culture &amp; Environment</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>ACCULT</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MACV</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>MEIM</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Acculturation Survey (PhenX Version)</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Mexican American Cultural Values Scale</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <t>Multigroup Ethnic Identity-Revised Survey</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIA</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vancouver Index of Acculturation</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>PBI</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>children's report of Parental Behavioral Inventory</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>MNBS</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multidimensional Neglecful Behavior Scale</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parental Monitoring</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>PM</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>FES</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Family Environment Scale</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>PET</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pet Ownership</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>PBP</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peer Behavior Profile</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peer Network Health: protective scale</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>PNH</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPI</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resistance to Peer Influence</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAG</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>School Attendance and Grades</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRPF</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>School Risk and Protective Factors scale</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE Part 1</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Culture-related Measures</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE Part 2</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Family-related Measures</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE Part 3</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peers- and Family-related Measures</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE Part 4</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other CE-related Measures</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>PSB</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProSocial Behavior scale</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>WPS</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wills Problem Solving scale</t>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1389,53 +1532,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2154,7 +2304,7 @@
       <c r="B46" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2753,7 +2903,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2761,14 +2911,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65B1762-B52F-442E-BD82-BE3591F36004}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2781,31 +2932,168 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>300</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>303</v>
+      <c r="A2" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B5" s="29" t="s">
         <v>305</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish Step 12 & Update Step 3
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A6202-4B3A-468F-89B6-561E9C31D01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12467CBA-3F99-46F4-A05B-86330F7E7F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17535" yWindow="4740" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,900 +22,896 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="348">
   <si>
     <t>Rep</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Rec</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Raw</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Raw data</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of Account</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>NOA</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ODQ</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Online Dating Questionnaire</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Imp</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Imputed data</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Re-coded data</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SMAS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>bergen Social Media Addiction Scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>VGAS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Video Game Addiction Scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MPIQ</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone Involvement Questionnaire</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SMQ</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Social Media Questionnaire</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UM</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Use Most</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowErs</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>NOFE</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>NOFI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowIngs</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>TPD</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SOCial media apps</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>weekday</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>weekend</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekday</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekend day</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>School</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>School-related work</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>calculated value from open-answered STQ items</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>TPW</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Time Per Week</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>TyPical Day (prefix) or Time Per Day (postfix)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SUAB</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Reorg</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Re-organized data</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Comp</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Compare</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ALL</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>all avaiable waves in ABCD 5.0</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>S</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Mental Health</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Children Short Form (ABCD-version)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_NU</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_SS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BIS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Inhibition System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BAS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BAS_FS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Fun Seeking (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BAS_Drive</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Drive (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BAS_RR</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Reward Responsiveness (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Sum</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Sum Scores (when as postfix of variable names)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Peer Experiences Questionnaire</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Agg</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Vic</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PPS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Prodromal Psychosis Scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Sum</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - Total number of youth-reported psychotic-like experiences</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - The severity score of PPS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Mania </t>
   </si>
   <si>
     <t>7-Up Mania Inventory</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Summary (when as postfix of files)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Negative Urgency (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Planning (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPers</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPlan</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Perseverance(Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_PU</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Positive Urgency (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Sensation Seeking (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity_Mean</t>
   </si>
   <si>
     <t>PPS Derivatives - The mean severity score of PPS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Youth-reported Life Events</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good_Affected</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad_Affected</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of bad events</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of good events</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of good events</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of bad events</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>T0</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SMA</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Screen Media Activity</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>T1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>OS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>OwnerShip</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>T2</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>STQ</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Screen Time Questionnaire</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>T3</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>T4</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MVA</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Missing Value Analysis</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Multiple Imputation</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SOC</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MVOC</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Multiplayer Videogame Online Chatting</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MP</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>One-year follow-up wave</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Two-year follow-up wave</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Three-year follow-up wave</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Four-year follow-up wave</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Baseline wave</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>auto-generated Report</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MH</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ERQ</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Emotion Regulation Questionnaire</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Reappraisal</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: reapprasial (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: Suppression (Sum Score)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Suppression</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>P</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Parent-reported About Youth</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Youth Self-reported</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Child Behavior Checklist</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Thought</t>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Thought Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Attention</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Attention Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>RuleBreak</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Aggressive</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Internal</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Internealizing Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>External</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Externalizing Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>TotProb</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Total Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Depress</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Anxitey</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Anxiety Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Somatic Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ADHD</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Attention Deficit/Hyperactivity Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Opposite</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Oppositional Defiant Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Conduct</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Conduct Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ASEBA</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Achenbach System of Empirically Based Assessment</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Aggressive Behavior</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Rule-breaking Behavior</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Social</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Social Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SomaticPr</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SomaticCo</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>WithDep</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Withdrawn/Depressed</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Somatic Complaints</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>AnxDep</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrom Scale - Anxious/Depressed</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SCT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>OCD</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Stress</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Sluggish Cognitive Tempo</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Obsessive-Compulsive Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Affective Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Post-traumatic Stress Problems</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>VSO</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Variable-values Summary Overview</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>NC</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Neuro-Cognition</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SU</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Magnetic Resonance Imaging</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>rsfMRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state functional MRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>tfMRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Task-based functional MRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>sMRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Structural MRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>DTI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Diffusion Tensor Imaging</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>RSI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Restriction Spectrum Imaging</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Quality Control of MRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>RecInc</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Recommended Image Inclusion</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>HM</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Head Motion</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MeanFD</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Mean Frame-wise Displacement</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MID</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Monetary Incentive Delay task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SST</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Stop Signal Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Behav</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Performance during task-based fMRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>QC</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>RSFNC</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state Functional canonical Network Connectivity</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CE</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Culture and Environment</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PH</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Physical Health</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Substance Use</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Ge</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Genetics</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>LED</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Linked External Data</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>NIHTB</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>The NIH Cognition Toolbox</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PVT</t>
   </si>
   <si>
     <t>Picture Vocabulary Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>FICAT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PSMT</t>
@@ -925,7 +921,7 @@
   </si>
   <si>
     <t>PCST</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ORRT</t>
@@ -941,445 +937,487 @@
   </si>
   <si>
     <t>Cryst</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Crystalized Intelligence Composite Score</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Fluid Intelligence Composite Score</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Total Intelligence Composite Score</t>
   </si>
   <si>
     <t>Flanker Inhibitory Control &amp; Attention Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> List Sorting Working Memory Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Oral Reading Recognition Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Pattern Comparison processing Speed Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Dimensional Change Card Sort Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Picture Sequence Memory Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Non-NIHTB</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognitive Task exlcuding NIH toolbox</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CCT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Cash Choice Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>LMT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Little Man Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>RAVLT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>the pearson Rey Auditory Verbal Learning Test</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>WISC</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Wechsler Intelligence Scale for Children (5th Ed.) - Martix Reasoning</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>DDT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Delay Discounting Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>EST</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Emotional Stroop Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>GDT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Game of Dice Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SIT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Social Influence Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SMART</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Stanford Mental Arithmetic Response Time Evaluation</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BIRD</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Indicator of Resiliency to Distress Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Millisecond Flanker Task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>NAA</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition Assessment Administration</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SVS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Snellen Visual Screener</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Common</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SDPP Derivatives File Name</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Novel Technology</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ABCD MRI-related Measures</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MRI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Screen</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Youth Mental Health Summary</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ABCD ASEBA Measures</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Abbr ASEBA</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MHS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Abbr NC</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>NB</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>emotional N-Back task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Activation System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Relational (Aggression or Victimization)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Reputational (Aggression or Victimization)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Overt (Aggression or Victimization)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>RECMEM</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>N-Back Recognition Memory task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MIDPQ</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Post-scan Questionnaire after MID task</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>FLKR</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>BDEFS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Barkely Deficits in Executive Functioning Scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Overt</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Rel</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Rep</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Aggression (only as postfix)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Victimization (only as postfix)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Abbr CE</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Culture &amp; Environment</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ACCULT</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MACV</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MEIM</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Acculturation Survey (PhenX Version)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Mexican American Cultural Values Scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Multigroup Ethnic Identity-Revised Survey</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>VIA</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Vancouver Index of Acculturation</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PBI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>children's report of Parental Behavioral Inventory</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>MNBS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Multidimensional Neglecful Behavior Scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Parental Monitoring</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PM</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>FES</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Family Environment Scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PET</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Pet Ownership</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PBP</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Peer Behavior Profile</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Peer Network Health: protective scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PNH</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>RPI</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Resistance to Peer Influence</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SAG</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>School Attendance and Grades</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>SRPF</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>School Risk and Protective Factors scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 1</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Culture-related Measures</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 2</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Family-related Measures</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 3</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Peers- and Family-related Measures</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 4</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Other CE-related Measures</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>PSB</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>ProSocial Behavior scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>WPS</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>Wills Problem Solving scale</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>dMRI</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diffusion MRI</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1w</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Structural MRI - T1-weighted Imaging</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Structural MRI - T2-weighted Imaging</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2w</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resting state fMRI - Temporal Variance</t>
+  </si>
+  <si>
+    <t>FNC</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>TVAR</t>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1496,6 +1534,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF444444"/>
+      <name val="Inter"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1532,60 +1576,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1815,11 +1862,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.125" bestFit="1" customWidth="1"/>
@@ -1829,27 +1876,27 @@
     <col min="6" max="6" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>96</v>
       </c>
@@ -1869,7 +1916,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>99</v>
       </c>
@@ -1882,14 +1929,14 @@
       <c r="D3" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="33" t="s">
         <v>195</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>102</v>
       </c>
@@ -1909,7 +1956,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>105</v>
       </c>
@@ -1929,7 +1976,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>106</v>
       </c>
@@ -1949,7 +1996,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>107</v>
       </c>
@@ -1962,14 +2009,14 @@
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>109</v>
       </c>
@@ -1983,13 +2030,13 @@
         <v>31</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="14" t="s">
         <v>177</v>
       </c>
@@ -2009,7 +2056,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -2022,14 +2069,14 @@
       <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
@@ -2042,14 +2089,14 @@
       <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -2062,14 +2109,14 @@
       <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -2082,14 +2129,14 @@
       <c r="D13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>205</v>
+      <c r="E13" s="15" t="s">
+        <v>192</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -2102,14 +2149,14 @@
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -2122,14 +2169,14 @@
       <c r="D15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
@@ -2142,8 +2189,14 @@
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -2156,8 +2209,14 @@
       <c r="D17" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="10" t="s">
         <v>129</v>
       </c>
@@ -2170,8 +2229,14 @@
       <c r="D18" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="10" t="s">
         <v>131</v>
       </c>
@@ -2184,8 +2249,14 @@
       <c r="D19" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
         <v>97</v>
       </c>
@@ -2199,7 +2270,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>122</v>
       </c>
@@ -2213,7 +2284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="11" t="s">
         <v>157</v>
       </c>
@@ -2227,7 +2298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="15" t="s">
         <v>179</v>
       </c>
@@ -2235,7 +2306,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="15" t="s">
         <v>182</v>
       </c>
@@ -2243,47 +2314,47 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B25" s="16" t="s">
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="15" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="15" t="s">
         <v>181</v>
       </c>
       <c r="B27" s="16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="15" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="B28" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B28" s="16" t="s">
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="15" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
         <v>61</v>
       </c>
@@ -2291,20 +2362,20 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2">
       <c r="B43" s="15"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2">
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2">
       <c r="B45" s="15"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2">
       <c r="B46" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2318,7 +2389,7 @@
       <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.125" bestFit="1" customWidth="1"/>
@@ -2328,32 +2399,32 @@
     <col min="6" max="6" width="64.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="B2" s="17" t="s">
         <v>220</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>221</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>52</v>
@@ -2368,18 +2439,18 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>223</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>168</v>
@@ -2388,12 +2459,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>55</v>
@@ -2408,12 +2479,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>57</v>
@@ -2428,12 +2499,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>59</v>
@@ -2448,12 +2519,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>63</v>
@@ -2468,18 +2539,18 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>137</v>
@@ -2488,18 +2559,18 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>139</v>
@@ -2508,18 +2579,18 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>233</v>
-      </c>
       <c r="C10" s="28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>140</v>
@@ -2528,18 +2599,18 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>141</v>
@@ -2548,18 +2619,18 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>143</v>
@@ -2568,12 +2639,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>242</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>243</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>67</v>
@@ -2588,12 +2659,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>267</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>268</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>69</v>
@@ -2608,12 +2679,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>244</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>245</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>71</v>
@@ -2628,12 +2699,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>246</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>247</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>84</v>
@@ -2648,12 +2719,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>248</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>249</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>73</v>
@@ -2668,12 +2739,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>250</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>251</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>48</v>
@@ -2688,12 +2759,12 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>252</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>253</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>78</v>
@@ -2708,12 +2779,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>254</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>255</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>79</v>
@@ -2728,12 +2799,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>256</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>257</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>50</v>
@@ -2748,12 +2819,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>258</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>259</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>81</v>
@@ -2768,12 +2839,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>260</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>261</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>51</v>
@@ -2782,12 +2853,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>262</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>263</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>87</v>
@@ -2796,12 +2867,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>88</v>
@@ -2810,12 +2881,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>291</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>292</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>89</v>
@@ -2824,12 +2895,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>265</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>266</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>90</v>
@@ -2838,7 +2909,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="22" t="s">
         <v>201</v>
       </c>
@@ -2852,7 +2923,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="22" t="s">
         <v>203</v>
       </c>
@@ -2866,12 +2937,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B30" s="23" t="s">
         <v>280</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>281</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>125</v>
@@ -2880,12 +2951,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>288</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>289</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>128</v>
@@ -2894,16 +2965,16 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="B32" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="B32" s="25" t="s">
-        <v>287</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2913,186 +2984,186 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65B1762-B52F-442E-BD82-BE3591F36004}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="B1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="29" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>328</v>
-      </c>
-      <c r="B2" s="32" t="s">
+      <c r="B3" s="29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="30" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="31" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>300</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>306</v>
-      </c>
-      <c r="B6" s="30" t="s">
+      <c r="B7" s="31" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="30" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>330</v>
-      </c>
-      <c r="B7" s="31" t="s">
+      <c r="B8" s="30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="31" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>310</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="B12" s="30" t="s">
+      <c r="B13" s="31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="30" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>332</v>
-      </c>
-      <c r="B13" s="31" t="s">
+      <c r="B14" s="30" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="31" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
-        <v>321</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
-        <v>322</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
-        <v>324</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
-        <v>326</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="B19" s="31" t="s">
         <v>334</v>
       </c>
-      <c r="B19" s="31" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="30" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
+      <c r="B20" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="B20" s="30" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="30" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
+      <c r="B21" s="30" t="s">
         <v>338</v>
       </c>
-      <c r="B21" s="30" t="s">
-        <v>339</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
accept multilple filter keys
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12467CBA-3F99-46F4-A05B-86330F7E7F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29376374-6646-4848-8438-769C57DCFD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="350">
   <si>
     <t>Rep</t>
     <phoneticPr fontId="15" type="noConversion"/>
@@ -1399,6 +1399,14 @@
   </si>
   <si>
     <t>TVAR</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abbr sMRI</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Structural Magnetic Resonance Imaging</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -1862,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2386,7 +2394,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2982,27 +2990,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65B1762-B52F-442E-BD82-BE3591F36004}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.75" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="20" t="s">
         <v>297</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="32" t="s">
         <v>327</v>
       </c>
@@ -3010,7 +3026,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" s="29" t="s">
         <v>299</v>
       </c>
@@ -3018,7 +3034,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" s="29" t="s">
         <v>300</v>
       </c>
@@ -3026,7 +3042,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5" s="29" t="s">
         <v>301</v>
       </c>
@@ -3034,7 +3050,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="A6" s="30" t="s">
         <v>305</v>
       </c>
@@ -3042,7 +3058,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4">
       <c r="A7" s="31" t="s">
         <v>329</v>
       </c>
@@ -3050,7 +3066,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="A8" s="30" t="s">
         <v>307</v>
       </c>
@@ -3058,7 +3074,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:4">
       <c r="A9" s="30" t="s">
         <v>309</v>
       </c>
@@ -3066,7 +3082,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:4">
       <c r="A10" s="30" t="s">
         <v>312</v>
       </c>
@@ -3074,7 +3090,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:4">
       <c r="A11" s="30" t="s">
         <v>313</v>
       </c>
@@ -3082,7 +3098,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4">
       <c r="A12" s="30" t="s">
         <v>315</v>
       </c>
@@ -3090,7 +3106,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:4">
       <c r="A13" s="31" t="s">
         <v>331</v>
       </c>
@@ -3098,7 +3114,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="A14" s="30" t="s">
         <v>317</v>
       </c>
@@ -3106,7 +3122,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:4">
       <c r="A15" s="30" t="s">
         <v>320</v>
       </c>
@@ -3114,7 +3130,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:4">
       <c r="A16" s="30" t="s">
         <v>321</v>
       </c>

</xml_diff>

<commit_message>
Finish Step 13, add step 14 & 15
</commit_message>
<xml_diff>
--- a/.github/SDPP_AbbrTable.xlsx
+++ b/.github/SDPP_AbbrTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ABCDStudyNDA\ABCD_DataAnalysis_5.0\SDPP_ABCD_TabulatedData\.github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29376374-6646-4848-8438-769C57DCFD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42B9731-262B-45BF-B661-C39F22DD6428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,896 +22,896 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="388">
   <si>
     <t>Rep</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Rec</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Raw</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Raw data</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of Account</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NOA</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ODQ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Online Dating Questionnaire</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Imp</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Imputed data</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Re-coded data</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SMAS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>bergen Social Media Addiction Scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>VGAS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Video Game Addiction Scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MPIQ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone Involvement Questionnaire</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SMQ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Social Media Questionnaire</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UM</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Use Most</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowErs</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NOFE</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NOFI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>the Number Of FollowIngs</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>TPD</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>open</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SOCial media apps</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>weekday</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>weekend</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekday</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>in a typical weekend day</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>School</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>School-related work</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>calculated value from open-answered STQ items</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>TPW</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Time Per Week</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>TyPical Day (prefix) or Time Per Day (postfix)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SUAB</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Screen Usage Around Bedtime</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Reorg</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Re-organized data</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Comp</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Compare</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ALL</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>all avaiable waves in ABCD 5.0</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>S</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Mental Health</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Children Short Form (ABCD-version)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_NU</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_SS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BIS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Inhibition System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BAS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BAS_FS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Fun Seeking (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BAS_Drive</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Drive (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BAS_RR</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BAS Subscale-Reward Responsiveness (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Sum</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Sum Scores (when as postfix of variable names)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Peer Experiences Questionnaire</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Agg</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Vic</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PPS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Prodromal Psychosis Scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Sum</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - Total number of youth-reported psychotic-like experiences</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PPS Derivatives - The severity score of PPS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Mania </t>
   </si>
   <si>
     <t>7-Up Mania Inventory</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Summary (when as postfix of files)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Negative Urgency (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Planning (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPers</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_LPlan</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Lack of Perseverance(Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS_PU</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Positive Urgency (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>UPPS-P Subscale - Sensation Seeking (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PPS_Severity_Mean</t>
   </si>
   <si>
     <t>PPS Derivatives - The mean severity score of PPS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Youth-reported Life Events</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Good_Affected</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE_Bad_Affected</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of bad events</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Total number of good events</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of good events</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>YLE Derivatives - Mean affected scores of bad events</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>T0</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SMA</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Screen Media Activity</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>T1</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>OS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>OwnerShip</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>T2</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>STQ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Screen Time Questionnaire</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>T3</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>T4</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MVA</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Missing Value Analysis</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Multiple Imputation</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SOC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MVOC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Multiplayer Videogame Online Chatting</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MP</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Mobile Phone</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>One-year follow-up wave</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Two-year follow-up wave</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Three-year follow-up wave</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Four-year follow-up wave</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Baseline wave</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>auto-generated Report</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MH</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ERQ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Emotion Regulation Questionnaire</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Reappraisal</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: reapprasial (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ERQ Subscale - emotion regulation strategies: Suppression (Sum Score)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ERQ_Suppression</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>P</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Parent-reported About Youth</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Youth Self-reported</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Child Behavior Checklist</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Thought</t>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Thought Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Attention</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Attention Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>RuleBreak</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Aggressive</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Internal</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Internealizing Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>External</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Externalizing Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>TotProb</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Composite Score - Total Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Depress</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Anxitey</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Anxiety Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Somatic Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ADHD</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Attention Deficit/Hyperactivity Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Opposite</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Oppositional Defiant Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Conduct</t>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Conduct Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ASEBA</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Achenbach System of Empirically Based Assessment</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Aggressive Behavior</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Rule-breaking Behavior</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Social</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Social Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SomaticPr</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SomaticCo</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>WithDep</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Withdrawn/Depressed</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrome Scale - Somatic Complaints</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>AnxDep</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL Syndrom Scale - Anxious/Depressed</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SCT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>OCD</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Stress</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Sluggish Cognitive Tempo</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Obsessive-Compulsive Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL DSM-5-Oriented Scale - Affective Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CBCL 2007 Scale - Post-traumatic Stress Problems</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>VSO</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Variable-values Summary Overview</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Neuro-Cognition</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SU</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Magnetic Resonance Imaging</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>rsfMRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state functional MRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>tfMRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Task-based functional MRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>sMRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Structural MRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>DTI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Diffusion Tensor Imaging</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>RSI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI - Restriction Spectrum Imaging</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Quality Control of MRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>RecInc</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Recommended Image Inclusion</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>HM</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Head Motion</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MeanFD</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Mean Frame-wise Displacement</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MID</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Monetary Incentive Delay task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SST</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Stop Signal Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Behav</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Performance during task-based fMRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>QC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Resting-state Functional canonical Network Connectivity</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CE</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Culture and Environment</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PH</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Physical Health</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Substance Use</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Ge</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Genetics</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>LED</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Linked External Data</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NIHTB</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>The NIH Cognition Toolbox</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PVT</t>
   </si>
   <si>
     <t>Picture Vocabulary Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>FICAT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PSMT</t>
@@ -921,7 +921,7 @@
   </si>
   <si>
     <t>PCST</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ORRT</t>
@@ -937,488 +937,653 @@
   </si>
   <si>
     <t>Cryst</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Crystalized Intelligence Composite Score</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Fluid Intelligence Composite Score</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Total Intelligence Composite Score</t>
   </si>
   <si>
     <t>Flanker Inhibitory Control &amp; Attention Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> List Sorting Working Memory Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Oral Reading Recognition Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Pattern Comparison processing Speed Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Dimensional Change Card Sort Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Picture Sequence Memory Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Non-NIHTB</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognitive Task exlcuding NIH toolbox</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CCT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Cash Choice Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>LMT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Little Man Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>RAVLT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>the pearson Rey Auditory Verbal Learning Test</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>WISC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Wechsler Intelligence Scale for Children (5th Ed.) - Martix Reasoning</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>DDT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Delay Discounting Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>EST</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Emotional Stroop Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>GDT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Game of Dice Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SIT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Social Influence Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SMART</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Stanford Mental Arithmetic Response Time Evaluation</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BIRD</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Indicator of Resiliency to Distress Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Millisecond Flanker Task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NAA</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Neurocognition Assessment Administration</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SVS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Snellen Visual Screener</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Common</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SDPP Derivatives File Name</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Novel Technology</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ABCD MRI-related Measures</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr Screen</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ABCD Youth Mental Health Summary</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ABCD ASEBA Measures</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr ASEBA</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr MHS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr NC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>NB</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>emotional N-Back task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Behavioral Activation System (subscale in BIS/BAS)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Relational (Aggression or Victimization)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Reputational (Aggression or Victimization)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Overt (Aggression or Victimization)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>RECMEM</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>N-Back Recognition Memory task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MIDPQ</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Post-scan Questionnaire after MID task</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>FLKR</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>BDEFS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Barkely Deficits in Executive Functioning Scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Overt</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Rel</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ_Rep</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Aggression (only as postfix)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PEQ Subscale - Dimension - Victimization (only as postfix)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr CE</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Culture &amp; Environment</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ACCULT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MACV</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MEIM</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Acculturation Survey (PhenX Version)</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Mexican American Cultural Values Scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Multigroup Ethnic Identity-Revised Survey</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>VIA</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Vancouver Index of Acculturation</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PBI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>children's report of Parental Behavioral Inventory</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>MNBS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Multidimensional Neglecful Behavior Scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Parental Monitoring</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PM</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>FES</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Family Environment Scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PET</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Pet Ownership</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PBP</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Peer Behavior Profile</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Peer Network Health: protective scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PNH</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>RPI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Resistance to Peer Influence</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SAG</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>School Attendance and Grades</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>SRPF</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>School Risk and Protective Factors scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 1</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Culture-related Measures</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 2</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Family-related Measures</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 3</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Peers- and Family-related Measures</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>CE Part 4</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Other CE-related Measures</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>PSB</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>ProSocial Behavior scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>WPS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Wills Problem Solving scale</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>dMRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Diffusion MRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>T1w</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Structural MRI - T1-weighted Imaging</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Structural MRI - T2-weighted Imaging</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>T2w</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Resting state fMRI - Temporal Variance</t>
   </si>
   <si>
     <t>FNC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>TVAR</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Abbr sMRI</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>Structural Magnetic Resonance Imaging</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>SULC</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>AREA</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOL</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cortical Thickness</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cortical surface Area</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cortical Sulcal depth</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>THICK</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average T1 intensity of gray matter voxels (+0.2 mm from ROI's gray/white boundary)</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average T2 intensity of white matter voxels (-0.2 mm from ROI's gray/white boundary)</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average T2 intensity of gray matter voxels (+0.2 mm from ROI's gray/white boundary)</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average T1 intensity of white matter voxels (-0.2 mm from ROI's gray/white boundary)</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normalized T1 cortical gray/white intensity contrast</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normalized T2 cortical gray/white intensity contrast</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>sMRI Part 1</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brain Morphometry</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>sMRI Part 2</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image intensity measures</t>
+  </si>
+  <si>
+    <t>sMRI Part 3</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regions of interest from Brain Atlas</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>labels from Desikan-Killiany atlas-based classification</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>labels from Destrieux atlas-based classification</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>lh</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>rh</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>left hemisphere</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>right hemisphere</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cortical or Subcortical Volume</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1Contr</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1Gray</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1White</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2Contr</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2Gray</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2White</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>DK</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean of vertex or voxel values in whole brain</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total value in whole brain</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1584,63 +1749,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2383,7 +2557,7 @@
       <c r="B46" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2982,7 +3156,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2990,18 +3164,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65B1762-B52F-442E-BD82-BE3591F36004}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.75" customWidth="1"/>
-    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
@@ -3025,6 +3199,12 @@
       <c r="B2" s="32" t="s">
         <v>328</v>
       </c>
+      <c r="C2" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="29" t="s">
@@ -3033,6 +3213,12 @@
       <c r="B3" s="29" t="s">
         <v>302</v>
       </c>
+      <c r="C3" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="29" t="s">
@@ -3041,6 +3227,12 @@
       <c r="B4" s="29" t="s">
         <v>303</v>
       </c>
+      <c r="C4" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="29" t="s">
@@ -3049,6 +3241,12 @@
       <c r="B5" s="29" t="s">
         <v>304</v>
       </c>
+      <c r="C5" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="30" t="s">
@@ -3057,6 +3255,12 @@
       <c r="B6" s="30" t="s">
         <v>306</v>
       </c>
+      <c r="C6" s="37" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="31" t="s">
@@ -3065,6 +3269,12 @@
       <c r="B7" s="31" t="s">
         <v>330</v>
       </c>
+      <c r="C7" s="39" t="s">
+        <v>365</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="30" t="s">
@@ -3073,6 +3283,12 @@
       <c r="B8" s="30" t="s">
         <v>308</v>
       </c>
+      <c r="C8" s="40" t="s">
+        <v>377</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="30" t="s">
@@ -3081,6 +3297,12 @@
       <c r="B9" s="30" t="s">
         <v>310</v>
       </c>
+      <c r="C9" s="40" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="30" t="s">
@@ -3089,6 +3311,12 @@
       <c r="B10" s="30" t="s">
         <v>311</v>
       </c>
+      <c r="C10" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="30" t="s">
@@ -3097,6 +3325,12 @@
       <c r="B11" s="30" t="s">
         <v>314</v>
       </c>
+      <c r="C11" s="40" t="s">
+        <v>380</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="30" t="s">
@@ -3105,6 +3339,12 @@
       <c r="B12" s="30" t="s">
         <v>316</v>
       </c>
+      <c r="C12" s="40" t="s">
+        <v>381</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="31" t="s">
@@ -3113,6 +3353,12 @@
       <c r="B13" s="31" t="s">
         <v>332</v>
       </c>
+      <c r="C13" s="40" t="s">
+        <v>382</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="30" t="s">
@@ -3121,6 +3367,12 @@
       <c r="B14" s="30" t="s">
         <v>318</v>
       </c>
+      <c r="C14" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="30" t="s">
@@ -3129,6 +3381,12 @@
       <c r="B15" s="30" t="s">
         <v>319</v>
       </c>
+      <c r="C15" s="40" t="s">
+        <v>383</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="30" t="s">
@@ -3137,40 +3395,70 @@
       <c r="B16" s="30" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="30" t="s">
         <v>323</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="37" t="s">
+        <v>372</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="30" t="s">
         <v>325</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="37" t="s">
+        <v>373</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="31" t="s">
         <v>333</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="40" t="s">
+        <v>386</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="30" t="s">
         <v>335</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="40" t="s">
+        <v>387</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="30" t="s">
         <v>337</v>
       </c>
@@ -3178,8 +3466,11 @@
         <v>338</v>
       </c>
     </row>
+    <row r="22" spans="1:4">
+      <c r="D22" s="37"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>